<commit_message>
can add food now
</commit_message>
<xml_diff>
--- a/backend/data/macro_nutrients_p2.xlsx
+++ b/backend/data/macro_nutrients_p2.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H108"/>
+  <dimension ref="A1:H109"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -3069,9 +3069,35 @@
         <v>10</v>
       </c>
     </row>
+    <row r="109">
+      <c r="A109" t="str">
+        <v>mango</v>
+      </c>
+      <c r="B109" t="str">
+        <v/>
+      </c>
+      <c r="C109" t="str">
+        <v/>
+      </c>
+      <c r="D109" t="str">
+        <v/>
+      </c>
+      <c r="E109">
+        <v>60</v>
+      </c>
+      <c r="F109">
+        <v>15</v>
+      </c>
+      <c r="G109">
+        <v>0.4</v>
+      </c>
+      <c r="H109">
+        <v>0.8</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H108"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H109"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>